<commit_message>
feature(CSharpFormat): Finish sample CSharpOutputFormat
</commit_message>
<xml_diff>
--- a/inputDir/demo.xlsx
+++ b/inputDir/demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\DataConvert\inputDir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4A22246E-A572-4AD6-98D3-ED015A00070D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43351988-0806-4AD0-B7F6-24BCDA2D969F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="65">
   <si>
     <t>HEAD</t>
   </si>
@@ -186,10 +186,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>System.out.println("hello:" + arg0);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>f0:Func0&lt;String&gt;</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -262,15 +258,8 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>arg0.put("k",1);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>f00:Func0&lt;Map&lt;String, Integer&gt;&gt;</t>
     <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>return new HashMap&lt;&gt;();</t>
   </si>
   <si>
     <t>formula:int</t>
@@ -295,6 +284,11 @@
   </si>
   <si>
     <t>3:4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>var a = 0;
+var c = a + arg0;</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -860,8 +854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="V11" sqref="V11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -881,7 +875,8 @@
     <col min="13" max="13" width="28.5" customWidth="1"/>
     <col min="14" max="16" width="26.375" customWidth="1"/>
     <col min="17" max="17" width="27" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="14.875" customWidth="1"/>
+    <col min="18" max="18" width="28.125" customWidth="1"/>
+    <col min="19" max="19" width="14.875" customWidth="1"/>
     <col min="20" max="20" width="22.25" customWidth="1"/>
     <col min="21" max="22" width="26" customWidth="1"/>
     <col min="23" max="23" width="27.75" customWidth="1"/>
@@ -1021,7 +1016,7 @@
         <v>36</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L7" s="5" t="s">
         <v>32</v>
@@ -1033,37 +1028,37 @@
         <v>34</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="P7" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q7" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R7" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S7" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="S7" s="5" t="s">
-        <v>45</v>
-      </c>
       <c r="T7" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="U7" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="U7" s="5" t="s">
+      <c r="V7" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="W7" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="V7" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="W7" s="5" t="s">
-        <v>55</v>
-      </c>
       <c r="X7" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="Y7" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="Z7" s="5"/>
     </row>
@@ -1093,19 +1088,48 @@
       </c>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="5"/>
-      <c r="U8" s="5"/>
-      <c r="V8" s="5"/>
-      <c r="W8" s="5"/>
-      <c r="X8" s="5"/>
+      <c r="L8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="P8" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="R8" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S8" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="T8" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="U8" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="V8" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="W8" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="X8" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y8" s="5" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="9" spans="1:26" ht="28.5">
       <c r="A9">
@@ -1132,43 +1156,39 @@
       <c r="J9" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="K9" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="L9" s="5" t="s">
-        <v>39</v>
+      <c r="K9" s="5"/>
+      <c r="L9" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
-      <c r="O9" s="8" t="s">
-        <v>60</v>
-      </c>
+      <c r="O9" s="8"/>
       <c r="P9" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q9" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R9" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="S9" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="S9" s="5" t="s">
-        <v>47</v>
-      </c>
       <c r="T9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="U9" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="U9" s="5" t="s">
-        <v>52</v>
-      </c>
       <c r="V9" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="W9" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="X9" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="Y9" s="5">
         <f>1451*6500005</f>
@@ -1211,7 +1231,7 @@
       <c r="T10" s="5"/>
       <c r="U10" s="5"/>
       <c r="V10" s="9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="W10" s="5"/>
       <c r="X10" s="5"/>
@@ -1874,17 +1894,17 @@
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>